<commit_message>
Fixat dataframe till bostadspriser och gjort en df
Ska försöka slå ihop de till en df och sedan skapa en funktion som visar
det användaren vill ha i en input. T.ex. "Mellan vilka år?" eller
liknande.
</commit_message>
<xml_diff>
--- a/Bostadspriser.xlsx
+++ b/Bostadspriser.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcus Turesson\Desktop\PythonProject4School\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E6E1639F-EF52-45B7-8058-09FEA4B9C7C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE5135E1-BBAF-430E-BB3C-8E220E3242B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,46 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
-  <si>
-    <t>1975</t>
-  </si>
-  <si>
-    <t>1976</t>
-  </si>
-  <si>
-    <t>1977</t>
-  </si>
-  <si>
-    <t>1978</t>
-  </si>
-  <si>
-    <t>1979</t>
-  </si>
-  <si>
-    <t>1980</t>
-  </si>
-  <si>
-    <t>1981</t>
-  </si>
-  <si>
-    <t>1982</t>
-  </si>
-  <si>
-    <t>1983</t>
-  </si>
-  <si>
-    <t>1984</t>
-  </si>
-  <si>
-    <t>1985</t>
-  </si>
-  <si>
-    <t>1986</t>
-  </si>
-  <si>
-    <t>1987</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>1988</t>
   </si>
@@ -532,7 +493,7 @@
   <dimension ref="A1:M50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -546,19 +507,19 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -574,16 +535,16 @@
         <v>0</v>
       </c>
       <c r="B2" s="2">
-        <v>59</v>
+        <v>154</v>
       </c>
       <c r="C2" s="2">
-        <v>53</v>
+        <v>189</v>
       </c>
       <c r="D2" s="2">
-        <v>62</v>
+        <v>181</v>
       </c>
       <c r="E2" s="2">
-        <v>58</v>
+        <v>157</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -599,16 +560,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>68</v>
+        <v>181</v>
       </c>
       <c r="C3" s="2">
-        <v>62</v>
+        <v>224</v>
       </c>
       <c r="D3" s="2">
-        <v>72</v>
+        <v>217</v>
       </c>
       <c r="E3" s="2">
-        <v>70</v>
+        <v>195</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -624,16 +585,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="2">
-        <v>79</v>
+        <v>203</v>
       </c>
       <c r="C4" s="2">
-        <v>71</v>
+        <v>247</v>
       </c>
       <c r="D4" s="2">
-        <v>83</v>
+        <v>242</v>
       </c>
       <c r="E4" s="2">
-        <v>80</v>
+        <v>229</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -649,16 +610,16 @@
         <v>3</v>
       </c>
       <c r="B5" s="2">
-        <v>89</v>
+        <v>217</v>
       </c>
       <c r="C5" s="2">
-        <v>83</v>
+        <v>254</v>
       </c>
       <c r="D5" s="2">
-        <v>92</v>
+        <v>253</v>
       </c>
       <c r="E5" s="2">
-        <v>91</v>
+        <v>258</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -674,16 +635,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="2">
-        <v>98</v>
+        <v>197</v>
       </c>
       <c r="C6" s="2">
-        <v>94</v>
+        <v>217</v>
       </c>
       <c r="D6" s="2">
-        <v>101</v>
+        <v>219</v>
       </c>
       <c r="E6" s="2">
-        <v>101</v>
+        <v>231</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -699,16 +660,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="2">
-        <v>101</v>
+        <v>175</v>
       </c>
       <c r="C7" s="2">
-        <v>100</v>
+        <v>184</v>
       </c>
       <c r="D7" s="2">
-        <v>104</v>
+        <v>189</v>
       </c>
       <c r="E7" s="2">
-        <v>102</v>
+        <v>197</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -724,16 +685,16 @@
         <v>6</v>
       </c>
       <c r="B8" s="2">
-        <v>100</v>
+        <v>183</v>
       </c>
       <c r="C8" s="2">
-        <v>100</v>
+        <v>202</v>
       </c>
       <c r="D8" s="2">
-        <v>100</v>
+        <v>199</v>
       </c>
       <c r="E8" s="2">
-        <v>100</v>
+        <v>208</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -749,16 +710,16 @@
         <v>7</v>
       </c>
       <c r="B9" s="2">
-        <v>101</v>
+        <v>184</v>
       </c>
       <c r="C9" s="2">
-        <v>101</v>
+        <v>206</v>
       </c>
       <c r="D9" s="2">
-        <v>101</v>
+        <v>200</v>
       </c>
       <c r="E9" s="2">
-        <v>100</v>
+        <v>210</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -774,16 +735,16 @@
         <v>8</v>
       </c>
       <c r="B10" s="2">
-        <v>101</v>
+        <v>185</v>
       </c>
       <c r="C10" s="2">
-        <v>103</v>
+        <v>207</v>
       </c>
       <c r="D10" s="2">
-        <v>104</v>
+        <v>201</v>
       </c>
       <c r="E10" s="2">
-        <v>100</v>
+        <v>213</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -799,16 +760,16 @@
         <v>9</v>
       </c>
       <c r="B11" s="2">
-        <v>105</v>
+        <v>198</v>
       </c>
       <c r="C11" s="2">
-        <v>105</v>
+        <v>233</v>
       </c>
       <c r="D11" s="2">
-        <v>110</v>
+        <v>220</v>
       </c>
       <c r="E11" s="2">
-        <v>105</v>
+        <v>230</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -824,16 +785,16 @@
         <v>10</v>
       </c>
       <c r="B12" s="2">
-        <v>109</v>
+        <v>217</v>
       </c>
       <c r="C12" s="2">
-        <v>111</v>
+        <v>269</v>
       </c>
       <c r="D12" s="2">
-        <v>116</v>
+        <v>249</v>
       </c>
       <c r="E12" s="2">
-        <v>109</v>
+        <v>261</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -849,16 +810,16 @@
         <v>11</v>
       </c>
       <c r="B13" s="2">
-        <v>115</v>
+        <v>237</v>
       </c>
       <c r="C13" s="2">
-        <v>121</v>
+        <v>308</v>
       </c>
       <c r="D13" s="2">
-        <v>126</v>
+        <v>274</v>
       </c>
       <c r="E13" s="2">
-        <v>114</v>
+        <v>302</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -874,16 +835,16 @@
         <v>12</v>
       </c>
       <c r="B14" s="2">
-        <v>130</v>
+        <v>263</v>
       </c>
       <c r="C14" s="2">
-        <v>148</v>
+        <v>374</v>
       </c>
       <c r="D14" s="2">
-        <v>148</v>
+        <v>305</v>
       </c>
       <c r="E14" s="2">
-        <v>129</v>
+        <v>346</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -899,16 +860,16 @@
         <v>13</v>
       </c>
       <c r="B15" s="2">
-        <v>154</v>
+        <v>284</v>
       </c>
       <c r="C15" s="2">
-        <v>189</v>
+        <v>411</v>
       </c>
       <c r="D15" s="2">
-        <v>181</v>
+        <v>328</v>
       </c>
       <c r="E15" s="2">
-        <v>157</v>
+        <v>374</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -924,16 +885,16 @@
         <v>14</v>
       </c>
       <c r="B16" s="2">
-        <v>181</v>
+        <v>302</v>
       </c>
       <c r="C16" s="2">
-        <v>224</v>
+        <v>434</v>
       </c>
       <c r="D16" s="2">
-        <v>217</v>
+        <v>351</v>
       </c>
       <c r="E16" s="2">
-        <v>195</v>
+        <v>403</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
@@ -949,16 +910,16 @@
         <v>15</v>
       </c>
       <c r="B17" s="2">
-        <v>203</v>
+        <v>322</v>
       </c>
       <c r="C17" s="2">
-        <v>247</v>
+        <v>443</v>
       </c>
       <c r="D17" s="2">
-        <v>242</v>
+        <v>394</v>
       </c>
       <c r="E17" s="2">
-        <v>229</v>
+        <v>445</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -974,16 +935,16 @@
         <v>16</v>
       </c>
       <c r="B18" s="2">
-        <v>217</v>
+        <v>353</v>
       </c>
       <c r="C18" s="2">
-        <v>254</v>
+        <v>475</v>
       </c>
       <c r="D18" s="2">
-        <v>253</v>
+        <v>446</v>
       </c>
       <c r="E18" s="2">
-        <v>258</v>
+        <v>503</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
@@ -999,16 +960,16 @@
         <v>17</v>
       </c>
       <c r="B19" s="2">
-        <v>197</v>
+        <v>387</v>
       </c>
       <c r="C19" s="2">
-        <v>217</v>
+        <v>509</v>
       </c>
       <c r="D19" s="2">
-        <v>219</v>
+        <v>505</v>
       </c>
       <c r="E19" s="2">
-        <v>231</v>
+        <v>569</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -1024,16 +985,16 @@
         <v>18</v>
       </c>
       <c r="B20" s="2">
-        <v>175</v>
+        <v>431</v>
       </c>
       <c r="C20" s="2">
-        <v>184</v>
+        <v>574</v>
       </c>
       <c r="D20" s="2">
-        <v>189</v>
+        <v>558</v>
       </c>
       <c r="E20" s="2">
-        <v>197</v>
+        <v>647</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
@@ -1049,16 +1010,16 @@
         <v>19</v>
       </c>
       <c r="B21" s="2">
-        <v>183</v>
+        <v>477</v>
       </c>
       <c r="C21" s="2">
-        <v>202</v>
+        <v>657</v>
       </c>
       <c r="D21" s="2">
-        <v>199</v>
+        <v>607</v>
       </c>
       <c r="E21" s="2">
-        <v>208</v>
+        <v>716</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
@@ -1074,16 +1035,16 @@
         <v>20</v>
       </c>
       <c r="B22" s="2">
-        <v>184</v>
+        <v>491</v>
       </c>
       <c r="C22" s="2">
-        <v>206</v>
+        <v>672</v>
       </c>
       <c r="D22" s="2">
-        <v>200</v>
+        <v>628</v>
       </c>
       <c r="E22" s="2">
-        <v>210</v>
+        <v>710</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
@@ -1099,16 +1060,16 @@
         <v>21</v>
       </c>
       <c r="B23" s="2">
-        <v>185</v>
+        <v>501</v>
       </c>
       <c r="C23" s="2">
-        <v>207</v>
+        <v>676</v>
       </c>
       <c r="D23" s="2">
-        <v>201</v>
+        <v>636</v>
       </c>
       <c r="E23" s="2">
-        <v>213</v>
+        <v>718</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
@@ -1124,16 +1085,16 @@
         <v>22</v>
       </c>
       <c r="B24" s="2">
-        <v>198</v>
+        <v>538</v>
       </c>
       <c r="C24" s="2">
-        <v>233</v>
+        <v>741</v>
       </c>
       <c r="D24" s="2">
-        <v>220</v>
+        <v>693</v>
       </c>
       <c r="E24" s="2">
-        <v>230</v>
+        <v>775</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
@@ -1149,16 +1110,16 @@
         <v>23</v>
       </c>
       <c r="B25" s="2">
-        <v>217</v>
+        <v>542</v>
       </c>
       <c r="C25" s="2">
-        <v>269</v>
+        <v>752</v>
       </c>
       <c r="D25" s="2">
-        <v>249</v>
+        <v>709</v>
       </c>
       <c r="E25" s="2">
-        <v>261</v>
+        <v>771</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
@@ -1174,16 +1135,16 @@
         <v>24</v>
       </c>
       <c r="B26" s="2">
-        <v>237</v>
+        <v>535</v>
       </c>
       <c r="C26" s="2">
-        <v>308</v>
+        <v>747</v>
       </c>
       <c r="D26" s="2">
-        <v>274</v>
+        <v>705</v>
       </c>
       <c r="E26" s="2">
-        <v>302</v>
+        <v>736</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
@@ -1199,16 +1160,16 @@
         <v>25</v>
       </c>
       <c r="B27" s="2">
-        <v>263</v>
+        <v>554</v>
       </c>
       <c r="C27" s="2">
-        <v>374</v>
+        <v>778</v>
       </c>
       <c r="D27" s="2">
-        <v>305</v>
+        <v>737</v>
       </c>
       <c r="E27" s="2">
-        <v>346</v>
+        <v>748</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
@@ -1224,16 +1185,16 @@
         <v>26</v>
       </c>
       <c r="B28" s="2">
-        <v>284</v>
+        <v>592</v>
       </c>
       <c r="C28" s="2">
-        <v>411</v>
+        <v>860</v>
       </c>
       <c r="D28" s="2">
-        <v>328</v>
+        <v>782</v>
       </c>
       <c r="E28" s="2">
-        <v>374</v>
+        <v>778</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
@@ -1249,16 +1210,16 @@
         <v>27</v>
       </c>
       <c r="B29" s="2">
-        <v>302</v>
+        <v>656</v>
       </c>
       <c r="C29" s="2">
-        <v>434</v>
+        <v>979</v>
       </c>
       <c r="D29" s="2">
-        <v>351</v>
+        <v>875</v>
       </c>
       <c r="E29" s="2">
-        <v>403</v>
+        <v>849</v>
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
@@ -1274,16 +1235,16 @@
         <v>28</v>
       </c>
       <c r="B30" s="2">
-        <v>322</v>
+        <v>711</v>
       </c>
       <c r="C30" s="2">
-        <v>443</v>
+        <v>1066</v>
       </c>
       <c r="D30" s="2">
-        <v>394</v>
+        <v>922</v>
       </c>
       <c r="E30" s="2">
-        <v>445</v>
+        <v>954</v>
       </c>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
@@ -1299,16 +1260,16 @@
         <v>29</v>
       </c>
       <c r="B31" s="2">
-        <v>353</v>
+        <v>770</v>
       </c>
       <c r="C31" s="2">
-        <v>475</v>
+        <v>1125</v>
       </c>
       <c r="D31" s="2">
-        <v>446</v>
+        <v>1022</v>
       </c>
       <c r="E31" s="2">
-        <v>503</v>
+        <v>1051</v>
       </c>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
@@ -1324,16 +1285,16 @@
         <v>30</v>
       </c>
       <c r="B32" s="2">
-        <v>387</v>
+        <v>770</v>
       </c>
       <c r="C32" s="2">
-        <v>509</v>
+        <v>1067</v>
       </c>
       <c r="D32" s="2">
-        <v>505</v>
+        <v>1014</v>
       </c>
       <c r="E32" s="2">
-        <v>569</v>
+        <v>1084</v>
       </c>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
@@ -1349,16 +1310,16 @@
         <v>31</v>
       </c>
       <c r="B33" s="2">
-        <v>431</v>
+        <v>791</v>
       </c>
       <c r="C33" s="2">
-        <v>574</v>
+        <v>1072</v>
       </c>
       <c r="D33" s="2">
-        <v>558</v>
+        <v>1045</v>
       </c>
       <c r="E33" s="2">
-        <v>647</v>
+        <v>1131</v>
       </c>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
@@ -1374,16 +1335,16 @@
         <v>32</v>
       </c>
       <c r="B34" s="2">
-        <v>477</v>
+        <v>843</v>
       </c>
       <c r="C34" s="2">
-        <v>657</v>
+        <v>1139</v>
       </c>
       <c r="D34" s="2">
-        <v>607</v>
+        <v>1098</v>
       </c>
       <c r="E34" s="2">
-        <v>716</v>
+        <v>1223</v>
       </c>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
@@ -1399,16 +1360,16 @@
         <v>33</v>
       </c>
       <c r="B35" s="2">
-        <v>491</v>
+        <v>985</v>
       </c>
       <c r="C35" s="2">
-        <v>672</v>
+        <v>1351</v>
       </c>
       <c r="D35" s="2">
-        <v>628</v>
+        <v>1271</v>
       </c>
       <c r="E35" s="2">
-        <v>710</v>
+        <v>1452</v>
       </c>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
@@ -1424,16 +1385,16 @@
         <v>34</v>
       </c>
       <c r="B36" s="2">
-        <v>501</v>
+        <v>1029</v>
       </c>
       <c r="C36" s="2">
-        <v>676</v>
+        <v>1399</v>
       </c>
       <c r="D36" s="2">
-        <v>636</v>
+        <v>1311</v>
       </c>
       <c r="E36" s="2">
-        <v>718</v>
+        <v>1491</v>
       </c>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
@@ -1449,16 +1410,16 @@
         <v>35</v>
       </c>
       <c r="B37" s="2">
-        <v>538</v>
+        <v>928</v>
       </c>
       <c r="C37" s="2">
-        <v>741</v>
+        <v>1246</v>
       </c>
       <c r="D37" s="2">
-        <v>693</v>
+        <v>1267</v>
       </c>
       <c r="E37" s="2">
-        <v>775</v>
+        <v>1323</v>
       </c>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
@@ -1470,21 +1431,6 @@
       <c r="M37" s="2"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B38" s="2">
-        <v>542</v>
-      </c>
-      <c r="C38" s="2">
-        <v>752</v>
-      </c>
-      <c r="D38" s="2">
-        <v>709</v>
-      </c>
-      <c r="E38" s="2">
-        <v>771</v>
-      </c>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
@@ -1495,21 +1441,6 @@
       <c r="M38" s="2"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A39" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B39" s="2">
-        <v>535</v>
-      </c>
-      <c r="C39" s="2">
-        <v>747</v>
-      </c>
-      <c r="D39" s="2">
-        <v>705</v>
-      </c>
-      <c r="E39" s="2">
-        <v>736</v>
-      </c>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
@@ -1520,21 +1451,6 @@
       <c r="M39" s="2"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B40" s="2">
-        <v>554</v>
-      </c>
-      <c r="C40" s="2">
-        <v>778</v>
-      </c>
-      <c r="D40" s="2">
-        <v>737</v>
-      </c>
-      <c r="E40" s="2">
-        <v>748</v>
-      </c>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
@@ -1545,21 +1461,6 @@
       <c r="M40" s="2"/>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A41" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B41" s="2">
-        <v>592</v>
-      </c>
-      <c r="C41" s="2">
-        <v>860</v>
-      </c>
-      <c r="D41" s="2">
-        <v>782</v>
-      </c>
-      <c r="E41" s="2">
-        <v>778</v>
-      </c>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
@@ -1570,21 +1471,6 @@
       <c r="M41" s="2"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A42" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B42" s="2">
-        <v>656</v>
-      </c>
-      <c r="C42" s="2">
-        <v>979</v>
-      </c>
-      <c r="D42" s="2">
-        <v>875</v>
-      </c>
-      <c r="E42" s="2">
-        <v>849</v>
-      </c>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
@@ -1595,21 +1481,6 @@
       <c r="M42" s="2"/>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A43" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B43" s="2">
-        <v>711</v>
-      </c>
-      <c r="C43" s="2">
-        <v>1066</v>
-      </c>
-      <c r="D43" s="2">
-        <v>922</v>
-      </c>
-      <c r="E43" s="2">
-        <v>954</v>
-      </c>
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
@@ -1620,21 +1491,6 @@
       <c r="M43" s="2"/>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A44" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B44" s="2">
-        <v>770</v>
-      </c>
-      <c r="C44" s="2">
-        <v>1125</v>
-      </c>
-      <c r="D44" s="2">
-        <v>1022</v>
-      </c>
-      <c r="E44" s="2">
-        <v>1051</v>
-      </c>
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
@@ -1645,21 +1501,6 @@
       <c r="M44" s="2"/>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A45" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B45" s="2">
-        <v>770</v>
-      </c>
-      <c r="C45" s="2">
-        <v>1067</v>
-      </c>
-      <c r="D45" s="2">
-        <v>1014</v>
-      </c>
-      <c r="E45" s="2">
-        <v>1084</v>
-      </c>
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
@@ -1670,21 +1511,6 @@
       <c r="M45" s="2"/>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A46" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B46" s="2">
-        <v>791</v>
-      </c>
-      <c r="C46" s="2">
-        <v>1072</v>
-      </c>
-      <c r="D46" s="2">
-        <v>1045</v>
-      </c>
-      <c r="E46" s="2">
-        <v>1131</v>
-      </c>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
@@ -1695,21 +1521,6 @@
       <c r="M46" s="2"/>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B47" s="2">
-        <v>843</v>
-      </c>
-      <c r="C47" s="2">
-        <v>1139</v>
-      </c>
-      <c r="D47" s="2">
-        <v>1098</v>
-      </c>
-      <c r="E47" s="2">
-        <v>1223</v>
-      </c>
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
@@ -1720,21 +1531,6 @@
       <c r="M47" s="2"/>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A48" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B48" s="2">
-        <v>985</v>
-      </c>
-      <c r="C48" s="2">
-        <v>1351</v>
-      </c>
-      <c r="D48" s="2">
-        <v>1271</v>
-      </c>
-      <c r="E48" s="2">
-        <v>1452</v>
-      </c>
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
@@ -1744,22 +1540,7 @@
       <c r="L48" s="2"/>
       <c r="M48" s="2"/>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A49" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B49" s="2">
-        <v>1029</v>
-      </c>
-      <c r="C49" s="2">
-        <v>1399</v>
-      </c>
-      <c r="D49" s="2">
-        <v>1311</v>
-      </c>
-      <c r="E49" s="2">
-        <v>1491</v>
-      </c>
+    <row r="49" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
@@ -1769,22 +1550,7 @@
       <c r="L49" s="2"/>
       <c r="M49" s="2"/>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A50" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B50" s="2">
-        <v>928</v>
-      </c>
-      <c r="C50" s="2">
-        <v>1246</v>
-      </c>
-      <c r="D50" s="2">
-        <v>1267</v>
-      </c>
-      <c r="E50" s="2">
-        <v>1323</v>
-      </c>
+    <row r="50" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>

</xml_diff>